<commit_message>
fix coaction ebs bug
</commit_message>
<xml_diff>
--- a/src/template.xlsx
+++ b/src/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awittung.2NDWATCH\PycharmProjects\CHscripts\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeversmeyer\Cloud Health\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883F37EC-0C07-4775-BE52-422010D185CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACA8E8B-3977-40EB-B5F0-A0E29FD5DFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42570" yWindow="4670" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>Account Name</t>
   </si>
@@ -552,30 +552,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09DC7943-7CD2-4B06-986F-7FD45C2BCD34}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -586,19 +586,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="7">
-        <f>SUM('EC2 Old Snapshots'!H2:H100000)</f>
+        <f>SUM('EC2 Old Snapshots'!G2:G100000)</f>
         <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -610,7 +610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -622,7 +622,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -634,7 +634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -646,7 +646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="174" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -655,7 +655,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -664,12 +664,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -685,26 +685,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.85546875" customWidth="1"/>
+    <col min="2" max="3" width="20.81640625" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,16 +723,13 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -751,20 +748,20 @@
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="22.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="7" max="7" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="22.26953125" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,21 +809,21 @@
       <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -874,17 +871,17 @@
       <selection pane="bottomLeft" activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,20 +919,20 @@
       <selection pane="bottomLeft" activeCell="J1" sqref="J1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -982,20 +979,20 @@
       <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="44.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" customWidth="1"/>
+    <col min="7" max="8" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7265625" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1034,21 +1031,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100178B648D21B7E3409B1165726F83F35C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="602a56321babd68959b332163c19152d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0ad01bea-cefe-40bb-967c-2cec37babb4c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e15dfd2ebf9896ba3bdf996c1dd12db" ns3:_="">
     <xsd:import namespace="0ad01bea-cefe-40bb-967c-2cec37babb4c"/>
@@ -1180,31 +1162,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F815069-03BF-4F0F-A43F-32B680C966B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA1B6C79-A680-4BAD-AF6F-A410C86047F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0ad01bea-cefe-40bb-967c-2cec37babb4c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D0357EC-28EF-4C58-9444-5BA3A085FE83}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1222,6 +1195,30 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA1B6C79-A680-4BAD-AF6F-A410C86047F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0ad01bea-cefe-40bb-967c-2cec37babb4c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F815069-03BF-4F0F-A43F-32B680C966B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{8242a0a9-c415-4206-be39-06637ad2817a}" enabled="0" method="" siteId="{8242a0a9-c415-4206-be39-06637ad2817a}" removed="1"/>

</xml_diff>